<commit_message>
Week 2 Time Sheet
</commit_message>
<xml_diff>
--- a/logs/GarciaRafael_1601Wk1_TimeEstimation.xlsx
+++ b/logs/GarciaRafael_1601Wk1_TimeEstimation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelgarcia/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelgarcia/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28340" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>RAFAEL MOSES GARCIA</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>ACTUAL TIME (Min)</t>
+  </si>
+  <si>
+    <t>Self Evaluation: SWOT</t>
+  </si>
+  <si>
+    <t>WK 2: Anchor Points</t>
+  </si>
+  <si>
+    <t>WK 2: Failure to Success</t>
+  </si>
+  <si>
+    <t>Mission Statement</t>
+  </si>
+  <si>
+    <t>WK 2: Project &amp; Portfolio</t>
   </si>
 </sst>
 </file>
@@ -202,7 +217,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -210,13 +225,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="60% - Accent1" xfId="4" builtinId="32"/>
@@ -498,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,12 +529,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -529,12 +545,12 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -545,12 +561,12 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="7">
         <v>1601</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -575,12 +591,12 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B7">
@@ -590,12 +606,12 @@
         <v>15</v>
       </c>
       <c r="D7" s="4">
-        <f>B7-C7</f>
+        <f t="shared" ref="D7:D12" si="0">B7-C7</f>
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B8">
@@ -605,12 +621,12 @@
         <v>15</v>
       </c>
       <c r="D8">
-        <f>B8-C8</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B9">
@@ -620,12 +636,12 @@
         <v>120</v>
       </c>
       <c r="D9">
-        <f>B9-C9</f>
+        <f t="shared" si="0"/>
         <v>-30</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B10">
@@ -635,12 +651,12 @@
         <v>260</v>
       </c>
       <c r="D10">
-        <f>B10-C10</f>
+        <f t="shared" si="0"/>
         <v>-80</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B11">
@@ -650,12 +666,12 @@
         <v>140</v>
       </c>
       <c r="D11">
-        <f>B11-C11</f>
+        <f t="shared" si="0"/>
         <v>-20</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B12">
@@ -665,7 +681,7 @@
         <v>170</v>
       </c>
       <c r="D12">
-        <f>B12-C12</f>
+        <f t="shared" si="0"/>
         <v>-50</v>
       </c>
     </row>
@@ -676,19 +692,101 @@
       <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:12" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B15">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="C15">
+        <v>45</v>
+      </c>
+      <c r="D15">
+        <f>B15-C15</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>60</v>
+      </c>
+      <c r="C16">
+        <v>70</v>
+      </c>
+      <c r="D16">
+        <f>B16-C16</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>45</v>
+      </c>
+      <c r="D17">
+        <f>B17-C17</f>
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>90</v>
+      </c>
+      <c r="C18">
+        <v>120</v>
+      </c>
+      <c r="D18">
+        <f>B18-C18</f>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>50</v>
+      </c>
+      <c r="D19">
+        <f>B19-C19</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>120</v>
+      </c>
+      <c r="C20">
+        <v>150</v>
+      </c>
+      <c r="D20">
+        <f>B20-C20</f>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A13:D13"/>

</xml_diff>